<commit_message>
UPDATE: datapreprocessing pca test
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>remake</t>
+          <t>Best Cinematography</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -451,7 +451,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>sequel</t>
+          <t xml:space="preserve"> Best Sound Mixing</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -461,7 +461,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>based on a true story</t>
+          <t>sports</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -471,7 +471,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>_august</t>
+          <t xml:space="preserve"> Best Supporting Actor</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -481,7 +481,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>_april</t>
+          <t xml:space="preserve"> Best Visual Effects</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -491,7 +491,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>period</t>
+          <t xml:space="preserve"> Cinematography</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -511,7 +511,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>horror</t>
+          <t>Writing (adapted screenplay)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -521,7 +521,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>adaptation</t>
+          <t>western</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -531,7 +531,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>screenplay</t>
+          <t>Visual Effects</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -541,7 +541,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>original</t>
+          <t xml:space="preserve"> Sound Editing</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -551,381 +551,901 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>sports</t>
+          <t xml:space="preserve"> Sound Mixing</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6.313638385686565e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>mystery</t>
+          <t>Costume Design</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6.865709246663202e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>_september</t>
+          <t>Best Supporting Actress (Patricia Arquette)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0002111755568490331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>fantasy</t>
+          <t>Best Supporting Actor (Jared Leto)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.001542873924331416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>_february</t>
+          <t>Best Supporting Actor</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.002496564360971142</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>_june</t>
+          <t>Best Film Editing</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002526173527991708</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>musical</t>
+          <t xml:space="preserve"> Production Design</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002563198118753674</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>thrilled</t>
+          <t xml:space="preserve"> Best Film Editing (Tom Cross)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.002654364202060568</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>_january</t>
+          <t>Best Actress (Cate Blanchett)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.003463546696318383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>history</t>
+          <t>fantasy</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.003519194002057682</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>war</t>
+          <t>sci-fi</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.003668614729892518</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>_july</t>
+          <t>_may</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.004779470842992843</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>_october</t>
+          <t>_march</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.005009510171515635</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>crime</t>
+          <t>period</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.006936487152046443</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>_march</t>
+          <t>crime</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.007245245031934726</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>_may</t>
+          <t xml:space="preserve"> Best Actor (Matthew McConaughey)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.007365802053876279</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>mystery</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.007488944819780281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>biography</t>
+          <t>_april</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.007900690582335416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>remake</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.009643692966293312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>adventure</t>
+          <t>_january</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.009995940744440988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>western</t>
+          <t>family</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.01102620198044317</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>comedy</t>
+          <t xml:space="preserve"> Best Cinematography</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.01111471395214925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>sci-fi</t>
+          <t>_february</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.01157779187554784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>_november</t>
+          <t>_august</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01252980933550101</v>
+        <v>6.357761134831232e-05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>drama</t>
+          <t>Best Supporting Actor (J.K. Simmons)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.0126600854486913</v>
+        <v>0.0001140432457568003</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>animation</t>
+          <t>thrilled</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.0130337840771673</v>
+        <v>0.0001668234954020425</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>romantic</t>
+          <t xml:space="preserve"> Best Makeup and Hairstyling (Adruitha Lee and Robin Mathews)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.01484475269622431</v>
+        <v>0.000380144152522669</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>_december</t>
+          <t>horror</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.01809379846085644</v>
+        <v>0.0003824117451385328</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>foreign gross</t>
+          <t xml:space="preserve"> Best Original Screenplay</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.02529127690582441</v>
+        <v>0.0004145747755971396</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>adventure</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.02995633927408201</v>
+        <v>0.0004172408513244529</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>budget recovered opening weekend</t>
+          <t>musical</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0493824571219856</v>
+        <v>0.0007123563873162332</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>budget ($million)</t>
+          <t>_october</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.06643371827282055</v>
+        <v>0.00114411205725164</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>opening weekend</t>
+          <t>action</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.07209571024212909</v>
+        <v>0.001186355060138209</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>imdb rating</t>
+          <t>Actor in a Leading Role</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.07579319630980838</v>
+        <v>0.001420115005115009</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>domestic gross</t>
+          <t>_july</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.09186465733453328</v>
+        <v>0.001717328583726326</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>budget recovered</t>
+          <t>_september</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.1119801304541397</v>
+        <v>0.001746772754914211</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>average audience</t>
+          <t>war</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.1356733119042677</v>
+        <v>0.001779618008305992</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Directing</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.00192229757209605</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>Best Actress</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.002020073346014945</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Sound</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.002358188125460815</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>_june</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.002437418473197094</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Writing (original screenplay)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.002871346710184615</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Animated Feature</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.00288908928879292</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Best Editing</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.002895040039130526</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>animation</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.002988747715731908</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>sequel</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.003071738319954514</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Adapted Screenplay</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.003521041232027668</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>romantic</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.00381649901292658</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>biography</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.003862568355657896</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Animated Feature Film</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.004581733264141152</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.004629564027753592</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>comedy</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.005386739866090491</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Make Up and Hair Styling</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.005690079913477174</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>adaptation</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.005713541297888588</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>Best Original Screenplay (Spike Jonze)</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.005957026300222758</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>_december</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.006131986705123058</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>drama</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.006355349585772363</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>_november</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.006532892570951632</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>Actress in a Leading Role</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.006860597745780897</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Sound Editing</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.006904829292818856</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Film Editing</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.007193430477572829</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ben Wilkins and Thomas Curley)</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.008057354748049269</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Best Adapted Screenplay</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.009321696364252462</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Best Actor</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.009876108434800527</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Best Visual Effects</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.01038297242312005</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0112231780820014</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Best Art Direction</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.01159541573716709</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Director</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.01165600125880912</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>history</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.01168590201064186</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Best Sound Mixing (Craig Mann</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.01232794899989588</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>based on a true story</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.01292636317925746</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Actress in a Supporting Role</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.01300496570237657</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Best Original Song</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.01487460327743167</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Best Director</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.01676189614991772</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Best Animated Film</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.01766508646193734</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Actor in a Supporting Role</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.01943641803447984</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>average audience</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.01951031273214117</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Original Song</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.02060409154272049</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Best Original Screenplay</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.02156405796495742</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>budget recovered</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.02640216761280089</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>budget recovered opening weekend</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0.0272123723899469</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>imdb rating</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.02834875769072259</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Best Supporting Actress</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.03784291968881236</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Best Picture</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.03962505381786232</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>budget ($million)</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.04819187672185874</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>domestic gross</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.04935033924180245</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>foreign gross</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0.05904429796412305</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>opening weekend</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0.06225877689308793</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Best Animated Feature</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.09260779311191843</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
           <t>average critics</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>0.1476235955217543</v>
+      <c r="B102" t="n">
+        <v>0.1584039787904806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>